<commit_message>
intermediate commit, working on utility/dollar for knapsack voting.
</commit_message>
<xml_diff>
--- a/data/mallows_utilities_voters=100_projects=4.xlsx
+++ b/data/mallows_utilities_voters=100_projects=4.xlsx
@@ -463,16 +463,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C2" t="n">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="D2" t="n">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="E2" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +482,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C3" t="n">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D3" t="n">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C4" t="n">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -520,16 +520,16 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>93</v>
+      </c>
+      <c r="C5" t="n">
+        <v>75</v>
+      </c>
+      <c r="D5" t="n">
         <v>91</v>
       </c>
-      <c r="C5" t="n">
-        <v>90</v>
-      </c>
-      <c r="D5" t="n">
-        <v>83</v>
-      </c>
       <c r="E5" t="n">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C6" t="n">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="D6" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
@@ -558,13 +558,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C7" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D7" t="n">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="E7" t="n">
         <v>26</v>
@@ -577,16 +577,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="C8" t="n">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E8" t="n">
-        <v>75</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
@@ -596,16 +596,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C9" t="n">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="E9" t="n">
-        <v>23</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
@@ -615,16 +615,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C10" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D10" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E10" t="n">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11">
@@ -634,16 +634,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="D11" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E11" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
@@ -653,16 +653,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="C12" t="n">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D12" t="n">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="E12" t="n">
-        <v>51</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
@@ -672,16 +672,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" t="n">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="D13" t="n">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E13" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
@@ -691,16 +691,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="C14" t="n">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="D14" t="n">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E14" t="n">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
@@ -710,16 +710,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="C15" t="n">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="D15" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D16" t="n">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -748,16 +748,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C17" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D17" t="n">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="E17" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="D18" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -786,16 +786,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="D19" t="n">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E19" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -805,16 +805,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="E20" t="n">
-        <v>50</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -824,16 +824,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="C21" t="n">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D21" t="n">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E21" t="n">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22">
@@ -843,16 +843,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C22" t="n">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="D22" t="n">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="E22" t="n">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23">
@@ -862,16 +862,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="C23" t="n">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="E23" t="n">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24">
@@ -881,16 +881,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C24" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" t="n">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="E24" t="n">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25">
@@ -900,16 +900,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="C25" t="n">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="D25" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E25" t="n">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26">
@@ -919,16 +919,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="C26" t="n">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="D26" t="n">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E26" t="n">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
@@ -938,16 +938,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C27" t="n">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="D27" t="n">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="E27" t="n">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28">
@@ -957,16 +957,16 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C28" t="n">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D28" t="n">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29">
@@ -976,16 +976,16 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="C29" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D29" t="n">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E29" t="n">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30">
@@ -995,16 +995,16 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="C30" t="n">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D30" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31">
@@ -1014,16 +1014,16 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C31" t="n">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="D31" t="n">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="E31" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
@@ -1033,16 +1033,16 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="C32" t="n">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="D32" t="n">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E32" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C33" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D33" t="n">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="E33" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34">
@@ -1071,16 +1071,16 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="D34" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35">
@@ -1090,16 +1090,16 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C35" t="n">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36">
@@ -1109,16 +1109,16 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C36" t="n">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="D36" t="n">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="E36" t="n">
-        <v>44</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37">
@@ -1128,16 +1128,16 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C37" t="n">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="D37" t="n">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="E37" t="n">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38">
@@ -1147,16 +1147,16 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C38" t="n">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="D38" t="n">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E38" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39">
@@ -1166,16 +1166,16 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D39" t="n">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="E39" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40">
@@ -1185,16 +1185,16 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C40" t="n">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D40" t="n">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="E40" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41">
@@ -1204,16 +1204,16 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C41" t="n">
         <v>78</v>
       </c>
       <c r="D41" t="n">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="E41" t="n">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C42" t="n">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="E42" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43">
@@ -1242,16 +1242,16 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C43" t="n">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D43" t="n">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="E43" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44">
@@ -1261,16 +1261,16 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D44" t="n">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="E44" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45">
@@ -1280,16 +1280,16 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D45" t="n">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="E45" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46">
@@ -1299,16 +1299,16 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C46" t="n">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="D46" t="n">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E46" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47">
@@ -1318,16 +1318,16 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C47" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="E47" t="n">
-        <v>36</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48">
@@ -1337,16 +1337,16 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C48" t="n">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="D48" t="n">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E48" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49">
@@ -1356,16 +1356,16 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C49" t="n">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="D49" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E49" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -1375,16 +1375,16 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C50" t="n">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="D50" t="n">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E50" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51">
@@ -1394,16 +1394,16 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C51" t="n">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="D51" t="n">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="E51" t="n">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52">
@@ -1413,16 +1413,16 @@
         </is>
       </c>
       <c r="B52" t="n">
+        <v>60</v>
+      </c>
+      <c r="C52" t="n">
+        <v>42</v>
+      </c>
+      <c r="D52" t="n">
+        <v>83</v>
+      </c>
+      <c r="E52" t="n">
         <v>69</v>
-      </c>
-      <c r="C52" t="n">
-        <v>83</v>
-      </c>
-      <c r="D52" t="n">
-        <v>75</v>
-      </c>
-      <c r="E52" t="n">
-        <v>38</v>
       </c>
     </row>
     <row r="53">
@@ -1432,16 +1432,16 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="C53" t="n">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D53" t="n">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="E53" t="n">
-        <v>19</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54">
@@ -1451,16 +1451,16 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C54" t="n">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="D54" t="n">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="E54" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55">
@@ -1470,16 +1470,16 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C55" t="n">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="D55" t="n">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E55" t="n">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56">
@@ -1489,16 +1489,16 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="C56" t="n">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="D56" t="n">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="E56" t="n">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57">
@@ -1508,16 +1508,16 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C57" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="E57" t="n">
-        <v>62</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58">
@@ -1527,16 +1527,16 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C58" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59">
@@ -1546,16 +1546,16 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C59" t="n">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="D59" t="n">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E59" t="n">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60">
@@ -1565,16 +1565,16 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C60" t="n">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="D60" t="n">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="E60" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61">
@@ -1584,16 +1584,16 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C61" t="n">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="D61" t="n">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="E61" t="n">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62">
@@ -1603,16 +1603,16 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D62" t="n">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="E62" t="n">
-        <v>36</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63">
@@ -1622,16 +1622,16 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C63" t="n">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="D63" t="n">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="E63" t="n">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64">
@@ -1641,16 +1641,16 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C64" t="n">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D64" t="n">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="E64" t="n">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65">
@@ -1660,16 +1660,16 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C65" t="n">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D65" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E65" t="n">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66">
@@ -1679,16 +1679,16 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C66" t="n">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D66" t="n">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E66" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67">
@@ -1698,16 +1698,16 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C67" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D67" t="n">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="E67" t="n">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68">
@@ -1717,16 +1717,16 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C68" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D68" t="n">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E68" t="n">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69">
@@ -1736,16 +1736,16 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="C69" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D69" t="n">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70">
@@ -1755,16 +1755,16 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="C70" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D70" t="n">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71">
@@ -1774,16 +1774,16 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C71" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D71" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E71" t="n">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72">
@@ -1793,16 +1793,16 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C72" t="n">
         <v>36</v>
       </c>
       <c r="D72" t="n">
+        <v>27</v>
+      </c>
+      <c r="E72" t="n">
         <v>82</v>
-      </c>
-      <c r="E72" t="n">
-        <v>48</v>
       </c>
     </row>
     <row r="73">
@@ -1812,16 +1812,16 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C73" t="n">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D73" t="n">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="E73" t="n">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74">
@@ -1831,16 +1831,16 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C74" t="n">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="D74" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E74" t="n">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75">
@@ -1850,16 +1850,16 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C75" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="D75" t="n">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76">
@@ -1869,16 +1869,16 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C76" t="n">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D76" t="n">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77">
@@ -1888,16 +1888,16 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="C77" t="n">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D77" t="n">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="E77" t="n">
-        <v>32</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78">
@@ -1907,16 +1907,16 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="C78" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D78" t="n">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="E78" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="79">
@@ -1926,16 +1926,16 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C79" t="n">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D79" t="n">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E79" t="n">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80">
@@ -1945,16 +1945,16 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C80" t="n">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="D80" t="n">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E80" t="n">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81">
@@ -1964,16 +1964,16 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C81" t="n">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D81" t="n">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E81" t="n">
-        <v>73</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82">
@@ -1983,16 +1983,16 @@
         </is>
       </c>
       <c r="B82" t="n">
+        <v>25</v>
+      </c>
+      <c r="C82" t="n">
         <v>61</v>
       </c>
-      <c r="C82" t="n">
-        <v>60</v>
-      </c>
       <c r="D82" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E82" t="n">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83">
@@ -2002,16 +2002,16 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C83" t="n">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D83" t="n">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E83" t="n">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84">
@@ -2021,16 +2021,16 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C84" t="n">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D84" t="n">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E84" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85">
@@ -2040,16 +2040,16 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="C85" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D85" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E85" t="n">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86">
@@ -2059,16 +2059,16 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C86" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D86" t="n">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="E86" t="n">
-        <v>63</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87">
@@ -2078,16 +2078,16 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C87" t="n">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="D87" t="n">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="E87" t="n">
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88">
@@ -2097,16 +2097,16 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="C88" t="n">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D88" t="n">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="E88" t="n">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89">
@@ -2116,16 +2116,16 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C89" t="n">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E89" t="n">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90">
@@ -2135,16 +2135,16 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C90" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D90" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E90" t="n">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91">
@@ -2154,16 +2154,16 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C91" t="n">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="D91" t="n">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E91" t="n">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="92">
@@ -2173,16 +2173,16 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C92" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D92" t="n">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="E92" t="n">
-        <v>50</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93">
@@ -2192,16 +2192,16 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C93" t="n">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="D93" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E93" t="n">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94">
@@ -2211,16 +2211,16 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C94" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D94" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E94" t="n">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="95">
@@ -2230,16 +2230,16 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D95" t="n">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="E95" t="n">
-        <v>19</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96">
@@ -2249,16 +2249,16 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C96" t="n">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D96" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E96" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="97">
@@ -2268,16 +2268,16 @@
         </is>
       </c>
       <c r="B97" t="n">
+        <v>0</v>
+      </c>
+      <c r="C97" t="n">
         <v>7</v>
       </c>
-      <c r="C97" t="n">
-        <v>11</v>
-      </c>
       <c r="D97" t="n">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="E97" t="n">
-        <v>68</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98">

</xml_diff>